<commit_message>
reading and import functionslity
</commit_message>
<xml_diff>
--- a/upload/excel_file/test.xlsx
+++ b/upload/excel_file/test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_R COMPUTERS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\test\upload\excel_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A92E8E-4C2A-4701-BDCC-377D36789EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8EBA34-E0CB-4FBC-BF45-4D9DC25EBEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +89,24 @@
   </si>
   <si>
     <t>Prod</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Mahindra</t>
+  </si>
+  <si>
+    <t>Shine</t>
+  </si>
+  <si>
+    <t>Badlapur</t>
   </si>
 </sst>
 </file>
@@ -418,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -539,4 +558,51 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97666CC9-74FE-46BA-88F8-7A1AA047026E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>